<commit_message>
Fixed and checked all navigation links
</commit_message>
<xml_diff>
--- a/chryswoods.com/vector_c++/diagrams.xlsx
+++ b/chryswoods.com/vector_c++/diagrams.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="0" windowWidth="28720" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="72">
   <si>
     <t>Register X</t>
   </si>
@@ -105,6 +105,144 @@
   </si>
   <si>
     <t>+</t>
+  </si>
+  <si>
+    <t>a[0]</t>
+  </si>
+  <si>
+    <t>a[1]</t>
+  </si>
+  <si>
+    <t>a[2]</t>
+  </si>
+  <si>
+    <t>a[3]</t>
+  </si>
+  <si>
+    <t>a[0] a[1] a[2] a[3]</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>a[20]</t>
+  </si>
+  <si>
+    <t>a[21]</t>
+  </si>
+  <si>
+    <t>a[22]</t>
+  </si>
+  <si>
+    <t>a[30]</t>
+  </si>
+  <si>
+    <t>a[31]</t>
+  </si>
+  <si>
+    <t>a[32]</t>
+  </si>
+  <si>
+    <t>a[40]</t>
+  </si>
+  <si>
+    <t>a[41]</t>
+  </si>
+  <si>
+    <t>a[42]</t>
+  </si>
+  <si>
+    <t>a[0] a[20] a[30] a[40]</t>
+  </si>
+  <si>
+    <t>a[0].x</t>
+  </si>
+  <si>
+    <t>a[0].y</t>
+  </si>
+  <si>
+    <t>a[0].z</t>
+  </si>
+  <si>
+    <t>a[1].x</t>
+  </si>
+  <si>
+    <t>a[2].y</t>
+  </si>
+  <si>
+    <t>a[1].z</t>
+  </si>
+  <si>
+    <t>a[2].x</t>
+  </si>
+  <si>
+    <t>a[2].z</t>
+  </si>
+  <si>
+    <t>a[1].y</t>
+  </si>
+  <si>
+    <t>a[3].x</t>
+  </si>
+  <si>
+    <t>a[3].y</t>
+  </si>
+  <si>
+    <t>a[3].z</t>
+  </si>
+  <si>
+    <t>a[0].x a[1].x a[2].x a[3].x</t>
+  </si>
+  <si>
+    <t>Vector Register</t>
+  </si>
+  <si>
+    <t>a.x[0]</t>
+  </si>
+  <si>
+    <t>a.x[1]</t>
+  </si>
+  <si>
+    <t>a.x[2]</t>
+  </si>
+  <si>
+    <t>a.x[3]</t>
+  </si>
+  <si>
+    <t>a.y[0]</t>
+  </si>
+  <si>
+    <t>a.y[1]</t>
+  </si>
+  <si>
+    <t>a.y[2]</t>
+  </si>
+  <si>
+    <t>a.y[3]</t>
+  </si>
+  <si>
+    <t>a.z[0]</t>
+  </si>
+  <si>
+    <t>a.z[1]</t>
+  </si>
+  <si>
+    <t>a.z[2]</t>
+  </si>
+  <si>
+    <t>a.z[3]</t>
+  </si>
+  <si>
+    <t>a.x[0] a.x[1] a.x[2] a.x[3]</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Aligned</t>
+  </si>
+  <si>
+    <t>Unaligned</t>
   </si>
 </sst>
 </file>
@@ -128,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,8 +285,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -156,11 +306,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -172,6 +359,43 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -635,6 +859,758 @@
         <a:xfrm flipH="1">
           <a:off x="12395200" y="4191001"/>
           <a:ext cx="1142999" cy="228599"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>16933</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2506133" y="8229600"/>
+          <a:ext cx="812800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>135467</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2514600" y="8348133"/>
+          <a:ext cx="1388533" cy="118534"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>16933</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>84666</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2506133" y="8348133"/>
+          <a:ext cx="1727200" cy="338667"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8467</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>448733</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2497667" y="8356600"/>
+          <a:ext cx="2099733" cy="499533"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2489200" y="9660467"/>
+          <a:ext cx="829733" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8467</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>592667</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>93133</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2497667" y="9770533"/>
+          <a:ext cx="1413933" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8467</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>169333</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2497667" y="9770533"/>
+          <a:ext cx="1820333" cy="1532467"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Arrow Connector 27"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2489200" y="9770533"/>
+          <a:ext cx="2192867" cy="2328334"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>16934</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Arrow Connector 32"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2489200" y="13521267"/>
+          <a:ext cx="846667" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8467</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>8467</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>668867</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Straight Arrow Connector 34"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2497667" y="13622867"/>
+          <a:ext cx="1490133" cy="499533"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>821266</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>8467</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>237066</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Arrow Connector 36"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2480733" y="13622867"/>
+          <a:ext cx="1905000" cy="1117600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>8467</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>626533</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Straight Arrow Connector 40"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2489200" y="13622867"/>
+          <a:ext cx="2286000" cy="1718733"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8467</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>821267</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>110068</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Straight Arrow Connector 42"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2497667" y="16569267"/>
+          <a:ext cx="812800" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>8467</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Straight Arrow Connector 45"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2489200" y="16670867"/>
+          <a:ext cx="1388533" cy="110066"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8467</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>186266</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>110067</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Straight Arrow Connector 47"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2497667" y="16679333"/>
+          <a:ext cx="1837266" cy="296334"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Straight Arrow Connector 49"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2489200" y="16679333"/>
+          <a:ext cx="2218267" cy="491067"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -926,10 +1902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B8:Q33"/>
+  <dimension ref="B8:Q114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A90" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -939,10 +1915,10 @@
   </cols>
   <sheetData>
     <row r="8" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="5"/>
       <c r="F8" s="1" t="s">
         <v>0</v>
       </c>
@@ -950,10 +1926,10 @@
       <c r="H8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="2"/>
+      <c r="M8" s="5"/>
       <c r="O8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1192,7 +2168,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:13" x14ac:dyDescent="0.2">
       <c r="K33" s="3" t="s">
         <v>24</v>
       </c>
@@ -1203,10 +2179,517 @@
         <v>18</v>
       </c>
     </row>
+    <row r="40" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C41" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C43" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C44" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C45" s="2"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C46" s="2"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C47" s="2"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C48" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C50" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C51" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C52" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C53" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C54" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C55" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C56" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56" s="6"/>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C57" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E57" s="6"/>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C58" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E58" s="6"/>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C59" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E59" s="6"/>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C60" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60" s="6"/>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C61" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E61" s="6"/>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C62" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E62" s="6"/>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C63" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E63" s="6"/>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E64" s="6"/>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="6"/>
+      <c r="E66" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C67" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F67" s="7"/>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C68" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C69" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C70" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C71" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C72" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C73" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C74" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C75" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C76" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C77" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C78" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C81" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" s="6"/>
+      <c r="E81" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C82" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E82" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F82" s="7"/>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C83" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="84" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C84" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C85" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C86" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C87" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C88" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C89" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C90" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C91" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C92" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C93" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C94" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="95" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C95" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="96" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C96" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B98" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C98" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B99" s="2">
+        <v>0</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B100" s="2">
+        <v>1</v>
+      </c>
+      <c r="C100" s="11"/>
+      <c r="D100" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B101" s="2">
+        <v>2</v>
+      </c>
+      <c r="C101" s="11"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B102" s="2">
+        <v>3</v>
+      </c>
+      <c r="C102" s="12"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B103" s="2">
+        <v>4</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D103" s="15"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B104" s="2">
+        <v>5</v>
+      </c>
+      <c r="C104" s="11"/>
+      <c r="D104" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E104" s="15"/>
+      <c r="F104" s="11"/>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B105" s="2">
+        <v>6</v>
+      </c>
+      <c r="C105" s="11"/>
+      <c r="D105" s="14"/>
+      <c r="E105" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F105" s="11"/>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B106" s="2">
+        <v>7</v>
+      </c>
+      <c r="C106" s="12"/>
+      <c r="D106" s="14"/>
+      <c r="E106" s="14"/>
+      <c r="F106" s="12"/>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B107" s="2">
+        <v>8</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D107" s="15"/>
+      <c r="E107" s="14"/>
+      <c r="F107" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B108" s="2">
+        <v>9</v>
+      </c>
+      <c r="C108" s="11"/>
+      <c r="D108" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E108" s="15"/>
+      <c r="F108" s="11"/>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B109" s="2">
+        <v>10</v>
+      </c>
+      <c r="C109" s="11"/>
+      <c r="D109" s="14"/>
+      <c r="E109" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F109" s="11"/>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B110" s="2">
+        <v>11</v>
+      </c>
+      <c r="C110" s="12"/>
+      <c r="D110" s="14"/>
+      <c r="E110" s="14"/>
+      <c r="F110" s="12"/>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B111" s="2">
+        <v>12</v>
+      </c>
+      <c r="C111" s="9"/>
+      <c r="D111" s="15"/>
+      <c r="E111" s="14"/>
+      <c r="F111" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B112" s="2">
+        <v>13</v>
+      </c>
+      <c r="C112" s="9"/>
+      <c r="E112" s="15"/>
+      <c r="F112" s="11"/>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B113" s="2">
+        <v>14</v>
+      </c>
+      <c r="C113" s="9"/>
+      <c r="F113" s="11"/>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B114" s="2">
+        <v>15</v>
+      </c>
+      <c r="C114" s="9"/>
+      <c r="F114" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="22">
+    <mergeCell ref="E101:E104"/>
+    <mergeCell ref="E105:E108"/>
+    <mergeCell ref="E109:E112"/>
+    <mergeCell ref="F103:F106"/>
+    <mergeCell ref="F107:F110"/>
+    <mergeCell ref="F111:F114"/>
+    <mergeCell ref="C99:C102"/>
+    <mergeCell ref="C103:C106"/>
+    <mergeCell ref="C107:C110"/>
+    <mergeCell ref="C111:C114"/>
+    <mergeCell ref="D100:D103"/>
+    <mergeCell ref="D104:D107"/>
+    <mergeCell ref="D108:D111"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E81:F81"/>
+    <mergeCell ref="E82:F82"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="L8:M8"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>